<commit_message>
budget updates for 2019 CSSI
</commit_message>
<xml_diff>
--- a/CSSI_2019/forms/CSSI_2019_Budget_AmyRoberts.xlsx
+++ b/CSSI_2019/forms/CSSI_2019_Budget_AmyRoberts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canto\Repositories\SI2.git\CSSI_2019\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CEF273-E5BC-46A7-9780-9609A6E4BDE6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AC64B1-3754-4967-96EB-0125CC7C0BD8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="98">
   <si>
     <t>On-Campus, Instruction 42%</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -237,9 +237,6 @@
     <t>Department:  Physics</t>
   </si>
   <si>
-    <t>Project Period:  07/01/2018-06/30/2021</t>
-  </si>
-  <si>
     <t>CY Contract (12 mo.)</t>
   </si>
   <si>
@@ -325,6 +322,15 @@
   </si>
   <si>
     <t>Project Title:  Elements: Improving tools based on data-description standards for gigabyte-scale data sets</t>
+  </si>
+  <si>
+    <t>cost per credit hour</t>
+  </si>
+  <si>
+    <t>" A computing device is considered a supply if the acquisition cost is less than the lesser of the capitalization level established by the proposer or $5,000, regardless of the length of its useful life. In the specific case of computing devices, charging as a direct cost is allowable for devices that are essential and allocable, but not solely dedicated, to the performance of the NSF project."</t>
+  </si>
+  <si>
+    <t>Project Period:  11/1/2019-10/30/2022</t>
   </si>
 </sst>
 </file>
@@ -928,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -945,7 +951,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -963,7 +969,7 @@
     </row>
     <row r="3" spans="1:12" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -972,7 +978,7 @@
     </row>
     <row r="4" spans="1:12" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1001,7 +1007,7 @@
         <v>38</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="13.9" x14ac:dyDescent="0.4">
@@ -1013,12 +1019,12 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="K7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="21">
         <f>$K8*1.03*10%*0</f>
@@ -1043,14 +1049,14 @@
     </row>
     <row r="9" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" s="9">
         <f>K9*0/10</f>
         <v>0</v>
       </c>
       <c r="C9" s="9">
-        <f t="shared" ref="C8:D10" si="1">B9*1.03</f>
+        <f t="shared" ref="C9:D10" si="1">B9*1.03</f>
         <v>0</v>
       </c>
       <c r="D9" s="9">
@@ -1067,7 +1073,7 @@
     </row>
     <row r="10" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="21">
         <f>K9*(1/9)</f>
@@ -1125,12 +1131,12 @@
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="K13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" s="9">
         <f>K14*0</f>
@@ -1153,36 +1159,36 @@
         <v>57591</v>
       </c>
       <c r="L14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="9">
         <f>K15*0.8</f>
-        <v>33600</v>
+        <v>34800</v>
       </c>
       <c r="C15" s="9">
         <f t="shared" ref="C15:D16" si="3">(B15*3%)+B15</f>
-        <v>34608</v>
+        <v>35844</v>
       </c>
       <c r="D15" s="9">
         <f t="shared" si="3"/>
-        <v>35646.239999999998</v>
+        <v>36919.32</v>
       </c>
       <c r="E15" s="18">
         <f t="shared" si="2"/>
-        <v>103854.23999999999</v>
+        <v>107563.32</v>
       </c>
       <c r="H15" s="32"/>
       <c r="I15" s="26"/>
       <c r="K15" s="17">
-        <v>42000</v>
+        <v>43500</v>
       </c>
       <c r="L15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
@@ -1227,7 +1233,7 @@
     </row>
     <row r="18" spans="1:14" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B18" s="9">
         <v>0</v>
@@ -1250,7 +1256,7 @@
         <v>47484</v>
       </c>
       <c r="L18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="13.5" x14ac:dyDescent="0.35">
@@ -1293,43 +1299,43 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20" t="s">
         <v>69</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>70</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>71</v>
-      </c>
-      <c r="N20" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" s="9">
         <f>K21*L21*M21*N21</f>
-        <v>11520</v>
+        <v>17280</v>
       </c>
       <c r="C21" s="9">
         <f t="shared" si="5"/>
-        <v>11865.6</v>
+        <v>17798.400000000001</v>
       </c>
       <c r="D21" s="9">
         <f t="shared" si="5"/>
-        <v>12221.568000000001</v>
+        <v>18332.352000000003</v>
       </c>
       <c r="E21" s="18">
         <f t="shared" si="2"/>
-        <v>35607.167999999998</v>
+        <v>53410.752000000008</v>
       </c>
       <c r="K21" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L21" s="17">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="M21" s="17">
         <v>32</v>
@@ -1340,7 +1346,7 @@
     </row>
     <row r="22" spans="1:14" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" s="9">
         <f>K22*L22*M22*N22</f>
@@ -1373,30 +1379,30 @@
     </row>
     <row r="23" spans="1:14" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="9">
         <f>K23*L23*M23*N23</f>
-        <v>9600</v>
+        <v>12000</v>
       </c>
       <c r="C23" s="9">
         <f t="shared" si="5"/>
-        <v>9888</v>
+        <v>12360</v>
       </c>
       <c r="D23" s="9">
         <f t="shared" si="5"/>
-        <v>10184.64</v>
+        <v>12730.8</v>
       </c>
       <c r="E23" s="18">
         <f t="shared" si="2"/>
-        <v>29672.639999999999</v>
+        <v>37090.800000000003</v>
       </c>
       <c r="F23" s="26"/>
       <c r="K23" s="17">
         <v>2</v>
       </c>
       <c r="L23" s="17">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M23" s="17">
         <v>32</v>
@@ -1407,7 +1413,7 @@
     </row>
     <row r="24" spans="1:14" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" s="9">
         <f>K24*L24*M24*N24</f>
@@ -1445,19 +1451,19 @@
       </c>
       <c r="B25" s="19">
         <f>SUM(B14:B24)</f>
-        <v>70200</v>
+        <v>79560</v>
       </c>
       <c r="C25" s="19">
         <f>SUM(C14:C24)</f>
-        <v>72306</v>
+        <v>81946.8</v>
       </c>
       <c r="D25" s="19">
         <f>SUM(D14:D24)</f>
-        <v>74475.179999999993</v>
+        <v>84405.204000000012</v>
       </c>
       <c r="E25" s="18">
         <f t="shared" si="2"/>
-        <v>216981.18</v>
+        <v>245912.00400000002</v>
       </c>
       <c r="G25" s="28"/>
     </row>
@@ -1479,7 +1485,7 @@
     </row>
     <row r="28" spans="1:14" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="18">
         <f>B11*27%</f>
@@ -1505,19 +1511,19 @@
       </c>
       <c r="B29" s="18">
         <f>SUM(B14+B15)*28%</f>
-        <v>9408</v>
+        <v>9744.0000000000018</v>
       </c>
       <c r="C29" s="18">
         <f>SUM(C14+C15)*28%</f>
-        <v>9690.2400000000016</v>
+        <v>10036.320000000002</v>
       </c>
       <c r="D29" s="18">
         <f>SUM(D14+D15)*28%</f>
-        <v>9980.9472000000005</v>
+        <v>10337.409600000001</v>
       </c>
       <c r="E29" s="18">
         <f t="shared" si="6"/>
-        <v>29079.1872</v>
+        <v>30117.729600000006</v>
       </c>
       <c r="H29" s="32"/>
       <c r="I29" s="26"/>
@@ -1640,19 +1646,19 @@
       </c>
       <c r="B35" s="18">
         <f>(B21+B23)*1%</f>
-        <v>211.20000000000002</v>
+        <v>292.8</v>
       </c>
       <c r="C35" s="18">
         <f>(C21+C23)*1%</f>
-        <v>217.536</v>
+        <v>301.584</v>
       </c>
       <c r="D35" s="18">
         <f>(D21+D23)*1%</f>
-        <v>224.06207999999998</v>
+        <v>310.63152000000002</v>
       </c>
       <c r="E35" s="18">
         <f t="shared" si="6"/>
-        <v>652.79808000000003</v>
+        <v>905.01552000000004</v>
       </c>
       <c r="F35" s="26"/>
     </row>
@@ -1684,19 +1690,19 @@
       </c>
       <c r="B37" s="19">
         <f>SUM(B28:B36)</f>
-        <v>11938.800000000001</v>
+        <v>12356.400000000001</v>
       </c>
       <c r="C37" s="19">
         <f>SUM(C28:C36)</f>
-        <v>12296.964000000002</v>
+        <v>12727.092000000004</v>
       </c>
       <c r="D37" s="19">
         <f>SUM(D28:D36)</f>
-        <v>14642.616063000001</v>
+        <v>15085.647903000003</v>
       </c>
       <c r="E37" s="18">
         <f t="shared" si="6"/>
-        <v>38878.380063000004</v>
+        <v>40169.13990300001</v>
       </c>
       <c r="F37" s="29"/>
       <c r="H37" s="29"/>
@@ -1714,19 +1720,19 @@
       </c>
       <c r="B39" s="19">
         <f>SUM(B11,B25,B37)</f>
-        <v>89583.244444444441</v>
+        <v>99360.844444444432</v>
       </c>
       <c r="C39" s="19">
         <f>SUM(C11,C25,C37)</f>
-        <v>92270.741777777788</v>
+        <v>102341.66977777779</v>
       </c>
       <c r="D39" s="19">
         <f>SUM(D11,D25,D37)</f>
-        <v>104336.8780741111</v>
+        <v>114709.93391411113</v>
       </c>
       <c r="E39" s="18">
         <f>SUM(B39:D39)</f>
-        <v>286190.86429633328</v>
+        <v>316412.44813633332</v>
       </c>
       <c r="F39" s="29"/>
       <c r="G39" s="28"/>
@@ -1753,17 +1759,17 @@
         <v>23</v>
       </c>
       <c r="B42" s="24">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="C42" s="24">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="D42" s="24">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="E42" s="18">
         <f>SUM(B42:D42)</f>
-        <v>3000</v>
+        <v>3600</v>
       </c>
       <c r="F42" s="27"/>
       <c r="G42" s="27"/>
@@ -1786,19 +1792,19 @@
       </c>
       <c r="B44" s="19">
         <f>SUM(B42:B43)</f>
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="C44" s="19">
         <f>SUM(C42:C43)</f>
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="D44" s="19">
         <f>SUM(D42:D43)</f>
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="E44" s="18">
         <f>SUM(B44:D44)</f>
-        <v>3000</v>
+        <v>3600</v>
       </c>
       <c r="F44" s="30"/>
       <c r="G44" s="30"/>
@@ -1826,13 +1832,16 @@
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
+      <c r="K46" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="47" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B47" s="9">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="C47" s="9">
         <v>4000</v>
@@ -1842,11 +1851,11 @@
       </c>
       <c r="E47" s="18">
         <f t="shared" ref="E47:E55" si="7">SUM(B47:D47)</f>
-        <v>12000</v>
+        <v>10000</v>
       </c>
       <c r="F47" s="26"/>
       <c r="K47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
@@ -1857,7 +1866,7 @@
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="18">
-        <f t="shared" si="7"/>
+        <f>SUM(B48:D48)</f>
         <v>0</v>
       </c>
     </row>
@@ -1946,7 +1955,7 @@
       </c>
       <c r="B55" s="19">
         <f>SUM(B47:B54)</f>
-        <v>4600</v>
+        <v>2600</v>
       </c>
       <c r="C55" s="19">
         <f>SUM(C47:C54)</f>
@@ -1958,7 +1967,7 @@
       </c>
       <c r="E55" s="18">
         <f t="shared" si="7"/>
-        <v>13800</v>
+        <v>11800</v>
       </c>
       <c r="F55" s="28"/>
     </row>
@@ -1980,14 +1989,16 @@
     </row>
     <row r="58" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A58" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B58" s="9"/>
+        <v>86</v>
+      </c>
+      <c r="B58" s="9">
+        <v>12204</v>
+      </c>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="18">
         <f t="shared" ref="E58:E69" si="8">SUM(B58:D58)</f>
-        <v>0</v>
+        <v>12204</v>
       </c>
       <c r="G58" s="26"/>
     </row>
@@ -2041,7 +2052,7 @@
         <v>10000</v>
       </c>
       <c r="E62" s="18">
-        <f t="shared" si="8"/>
+        <f>SUM(B62:D62)</f>
         <v>30000</v>
       </c>
     </row>
@@ -2081,7 +2092,10 @@
         <v>0</v>
       </c>
       <c r="K65" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="L65" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="40.5" x14ac:dyDescent="0.35">
@@ -2089,22 +2103,26 @@
         <v>63</v>
       </c>
       <c r="B66" s="9">
-        <v>10760</v>
+        <f>2*K66*L66</f>
+        <v>8952</v>
       </c>
       <c r="C66" s="9">
         <f>B66*1.05</f>
-        <v>11298</v>
+        <v>9399.6</v>
       </c>
       <c r="D66" s="9">
         <f>C66*1.05</f>
-        <v>11862.9</v>
+        <v>9869.58</v>
       </c>
       <c r="E66" s="18">
         <f t="shared" si="8"/>
-        <v>33920.9</v>
+        <v>28221.18</v>
       </c>
       <c r="K66">
         <v>12</v>
+      </c>
+      <c r="L66">
+        <v>373</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
@@ -2112,28 +2130,28 @@
         <v>35</v>
       </c>
       <c r="B67" s="9">
-        <v>16000</v>
+        <v>0</v>
       </c>
       <c r="C67" s="9">
         <f>B67*1.03</f>
-        <v>16480</v>
+        <v>0</v>
       </c>
       <c r="D67" s="9">
         <f>C67*1.03</f>
-        <v>16974.400000000001</v>
+        <v>0</v>
       </c>
       <c r="E67" s="18">
         <f t="shared" si="8"/>
-        <v>49454.400000000001</v>
+        <v>0</v>
       </c>
       <c r="K67" t="s">
+        <v>90</v>
+      </c>
+      <c r="L67" t="s">
         <v>91</v>
       </c>
-      <c r="L67" t="s">
-        <v>92</v>
-      </c>
       <c r="M67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
@@ -2173,19 +2191,19 @@
       </c>
       <c r="B69" s="19">
         <f>SUM(B58:B68)</f>
-        <v>41026</v>
+        <v>35422</v>
       </c>
       <c r="C69" s="19">
         <f>SUM(C58:C68)</f>
-        <v>42171.98</v>
+        <v>23793.579999999998</v>
       </c>
       <c r="D69" s="19">
         <f>SUM(D58:D68)</f>
-        <v>43363.099400000006</v>
+        <v>24395.379400000002</v>
       </c>
       <c r="E69" s="18">
         <f t="shared" si="8"/>
-        <v>126561.07940000002</v>
+        <v>83610.959400000007</v>
       </c>
       <c r="G69" s="26"/>
     </row>
@@ -2202,19 +2220,19 @@
       </c>
       <c r="B71" s="18">
         <f>B11+B25+B37+B44+B55-B51</f>
-        <v>95183.244444444441</v>
+        <v>103160.84444444443</v>
       </c>
       <c r="C71" s="18">
         <f>C11+C25+C37+C44+C55-C51</f>
-        <v>97870.741777777788</v>
+        <v>108141.66977777779</v>
       </c>
       <c r="D71" s="18">
         <f>D11+D25+D37+D44+D55-D51</f>
-        <v>109936.8780741111</v>
+        <v>120509.93391411113</v>
       </c>
       <c r="E71" s="18">
         <f>SUM(B71:D71)</f>
-        <v>302990.86429633328</v>
+        <v>331812.44813633332</v>
       </c>
       <c r="F71" s="26"/>
       <c r="G71" s="26"/>
@@ -2233,19 +2251,19 @@
       </c>
       <c r="B73" s="18">
         <f>B11+B25+B37+B44+B55+B69</f>
-        <v>136209.24444444443</v>
+        <v>138582.84444444443</v>
       </c>
       <c r="C73" s="18">
         <f>C11+C25+C37+C44+C55+C69</f>
-        <v>140042.7217777778</v>
+        <v>131935.24977777779</v>
       </c>
       <c r="D73" s="18">
         <f>D11+D25+D37+D44+D55+D69</f>
-        <v>153299.9774741111</v>
+        <v>144905.31331411112</v>
       </c>
       <c r="E73" s="18">
         <f>SUM(B73:D73)</f>
-        <v>429551.94369633333</v>
+        <v>415423.40753633331</v>
       </c>
       <c r="F73" s="26"/>
       <c r="G73" s="26"/>
@@ -2263,19 +2281,19 @@
       </c>
       <c r="B75" s="18">
         <f>B71*0.555</f>
-        <v>52826.700666666671</v>
+        <v>57254.268666666663</v>
       </c>
       <c r="C75" s="18">
         <f>C71*55.5%</f>
-        <v>54318.261686666679</v>
+        <v>60018.626726666676</v>
       </c>
       <c r="D75" s="18">
         <f>D71*55.5%</f>
-        <v>61014.967331131666</v>
+        <v>66883.013322331681</v>
       </c>
       <c r="E75" s="18">
         <f>SUM(B75:D75)</f>
-        <v>168159.92968446502</v>
+        <v>184155.90871566502</v>
       </c>
       <c r="F75" s="25"/>
       <c r="G75" s="25"/>
@@ -2294,19 +2312,19 @@
       </c>
       <c r="B77" s="18">
         <f>B73+B75</f>
-        <v>189035.9451111111</v>
+        <v>195837.1131111111</v>
       </c>
       <c r="C77" s="18">
         <f>C73+C75</f>
-        <v>194360.98346444446</v>
+        <v>191953.87650444446</v>
       </c>
       <c r="D77" s="18">
         <f>D73+D75</f>
-        <v>214314.94480524276</v>
+        <v>211788.3266364428</v>
       </c>
       <c r="E77" s="18">
         <f>SUM(B77:D77)</f>
-        <v>597711.87338079838</v>
+        <v>599579.3162519983</v>
       </c>
       <c r="F77" s="25"/>
       <c r="G77" s="25"/>

</xml_diff>

<commit_message>
further updates to budget for CSSI 2019
</commit_message>
<xml_diff>
--- a/CSSI_2019/forms/CSSI_2019_Budget_AmyRoberts.xlsx
+++ b/CSSI_2019/forms/CSSI_2019_Budget_AmyRoberts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canto\Repositories\SI2.git\CSSI_2019\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AC64B1-3754-4967-96EB-0125CC7C0BD8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6BC409-0F05-4734-8EB8-9822AA2BFE24}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -934,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1031,16 +1031,16 @@
         <v>0</v>
       </c>
       <c r="C8" s="21">
-        <f>$K8*1.03*1.03*10%*0</f>
-        <v>0</v>
+        <f>$K8*1.03*1.03*10%*1</f>
+        <v>7108.0300000000007</v>
       </c>
       <c r="D8" s="21">
-        <f>$K8*1.03*1.03*1.03*10%*1</f>
-        <v>7321.2709000000004</v>
+        <f>$K8*1.03*1.03*1.03*10%*0</f>
+        <v>0</v>
       </c>
       <c r="E8" s="18">
         <f t="shared" ref="E8:E11" si="0">SUM(B8:D8)</f>
-        <v>7321.2709000000004</v>
+        <v>7108.0300000000007</v>
       </c>
       <c r="F8" s="26"/>
       <c r="K8" s="17">
@@ -1076,20 +1076,20 @@
         <v>84</v>
       </c>
       <c r="B10" s="21">
-        <f>K9*(1/9)</f>
-        <v>7444.4444444444443</v>
+        <f>K9*(1/10)</f>
+        <v>6700</v>
       </c>
       <c r="C10" s="21">
         <f t="shared" si="1"/>
-        <v>7667.7777777777783</v>
+        <v>6901</v>
       </c>
       <c r="D10" s="21">
         <f t="shared" si="1"/>
-        <v>7897.811111111112</v>
+        <v>7108.03</v>
       </c>
       <c r="E10" s="18">
         <f t="shared" si="0"/>
-        <v>23010.033333333333</v>
+        <v>20709.03</v>
       </c>
       <c r="F10" s="26"/>
     </row>
@@ -1099,19 +1099,19 @@
       </c>
       <c r="B11" s="19">
         <f>SUM(B8:B10)</f>
-        <v>7444.4444444444443</v>
+        <v>6700</v>
       </c>
       <c r="C11" s="19">
         <f>SUM(C8:C10)</f>
-        <v>7667.7777777777783</v>
+        <v>14009.03</v>
       </c>
       <c r="D11" s="19">
         <f>SUM(D8:D10)</f>
-        <v>15219.082011111113</v>
+        <v>7108.03</v>
       </c>
       <c r="E11" s="18">
         <f t="shared" si="0"/>
-        <v>30331.304233333336</v>
+        <v>27817.059999999998</v>
       </c>
       <c r="F11" s="26"/>
     </row>
@@ -1168,24 +1168,24 @@
       </c>
       <c r="B15" s="9">
         <f>K15*0.8</f>
-        <v>34800</v>
+        <v>33600</v>
       </c>
       <c r="C15" s="9">
         <f t="shared" ref="C15:D16" si="3">(B15*3%)+B15</f>
-        <v>35844</v>
+        <v>34608</v>
       </c>
       <c r="D15" s="9">
         <f t="shared" si="3"/>
-        <v>36919.32</v>
+        <v>35646.239999999998</v>
       </c>
       <c r="E15" s="18">
         <f t="shared" si="2"/>
-        <v>107563.32</v>
+        <v>103854.23999999999</v>
       </c>
       <c r="H15" s="32"/>
       <c r="I15" s="26"/>
       <c r="K15" s="17">
-        <v>43500</v>
+        <v>42000</v>
       </c>
       <c r="L15" t="s">
         <v>81</v>
@@ -1350,22 +1350,22 @@
       </c>
       <c r="B22" s="9">
         <f>K22*L22*M22*N22</f>
-        <v>6480</v>
+        <v>12960</v>
       </c>
       <c r="C22" s="9">
         <f t="shared" si="5"/>
-        <v>6674.4</v>
+        <v>13348.8</v>
       </c>
       <c r="D22" s="9">
         <f t="shared" si="5"/>
-        <v>6874.6319999999996</v>
+        <v>13749.263999999999</v>
       </c>
       <c r="E22" s="18">
         <f t="shared" si="2"/>
-        <v>20029.031999999999</v>
+        <v>40058.063999999998</v>
       </c>
       <c r="K22" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L22" s="17">
         <v>30</v>
@@ -1383,26 +1383,26 @@
       </c>
       <c r="B23" s="9">
         <f>K23*L23*M23*N23</f>
-        <v>12000</v>
+        <v>8000</v>
       </c>
       <c r="C23" s="9">
         <f t="shared" si="5"/>
-        <v>12360</v>
+        <v>8240</v>
       </c>
       <c r="D23" s="9">
         <f t="shared" si="5"/>
-        <v>12730.8</v>
+        <v>8487.2000000000007</v>
       </c>
       <c r="E23" s="18">
         <f t="shared" si="2"/>
-        <v>37090.800000000003</v>
+        <v>24727.200000000001</v>
       </c>
       <c r="F23" s="26"/>
       <c r="K23" s="17">
         <v>2</v>
       </c>
       <c r="L23" s="17">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M23" s="17">
         <v>32</v>
@@ -1451,19 +1451,19 @@
       </c>
       <c r="B25" s="19">
         <f>SUM(B14:B24)</f>
-        <v>79560</v>
+        <v>80840</v>
       </c>
       <c r="C25" s="19">
         <f>SUM(C14:C24)</f>
-        <v>81946.8</v>
+        <v>83265.2</v>
       </c>
       <c r="D25" s="19">
         <f>SUM(D14:D24)</f>
-        <v>84405.204000000012</v>
+        <v>85763.156000000003</v>
       </c>
       <c r="E25" s="18">
         <f t="shared" si="2"/>
-        <v>245912.00400000002</v>
+        <v>249868.35600000003</v>
       </c>
       <c r="G25" s="28"/>
     </row>
@@ -1489,19 +1489,19 @@
       </c>
       <c r="B28" s="18">
         <f>B11*27%</f>
-        <v>2010</v>
+        <v>1809.0000000000002</v>
       </c>
       <c r="C28" s="18">
         <f>C11*27%</f>
-        <v>2070.3000000000002</v>
+        <v>3782.4381000000003</v>
       </c>
       <c r="D28" s="18">
         <f>D11*27%</f>
-        <v>4109.1521430000012</v>
+        <v>1919.1681000000001</v>
       </c>
       <c r="E28" s="18">
         <f t="shared" ref="E28:E37" si="6">SUM(B28:D28)</f>
-        <v>8189.4521430000013</v>
+        <v>7510.6062000000002</v>
       </c>
       <c r="F28" s="25"/>
     </row>
@@ -1511,19 +1511,19 @@
       </c>
       <c r="B29" s="18">
         <f>SUM(B14+B15)*28%</f>
-        <v>9744.0000000000018</v>
+        <v>9408</v>
       </c>
       <c r="C29" s="18">
         <f>SUM(C14+C15)*28%</f>
-        <v>10036.320000000002</v>
+        <v>9690.2400000000016</v>
       </c>
       <c r="D29" s="18">
         <f>SUM(D14+D15)*28%</f>
-        <v>10337.409600000001</v>
+        <v>9980.9472000000005</v>
       </c>
       <c r="E29" s="18">
         <f t="shared" si="6"/>
-        <v>30117.729600000006</v>
+        <v>29079.1872</v>
       </c>
       <c r="H29" s="32"/>
       <c r="I29" s="26"/>
@@ -1646,19 +1646,19 @@
       </c>
       <c r="B35" s="18">
         <f>(B21+B23)*1%</f>
-        <v>292.8</v>
+        <v>252.8</v>
       </c>
       <c r="C35" s="18">
         <f>(C21+C23)*1%</f>
-        <v>301.584</v>
+        <v>260.38400000000001</v>
       </c>
       <c r="D35" s="18">
         <f>(D21+D23)*1%</f>
-        <v>310.63152000000002</v>
+        <v>268.19552000000004</v>
       </c>
       <c r="E35" s="18">
         <f t="shared" si="6"/>
-        <v>905.01552000000004</v>
+        <v>781.37951999999996</v>
       </c>
       <c r="F35" s="26"/>
     </row>
@@ -1668,19 +1668,19 @@
       </c>
       <c r="B36" s="18">
         <f>(B22+B24)*2%</f>
-        <v>309.60000000000002</v>
+        <v>439.2</v>
       </c>
       <c r="C36" s="18">
         <f>(C22+C24)*2%</f>
-        <v>318.88799999999998</v>
+        <v>452.37599999999998</v>
       </c>
       <c r="D36" s="18">
         <f>(D22+D24)*2%</f>
-        <v>328.45463999999998</v>
+        <v>465.94728000000003</v>
       </c>
       <c r="E36" s="18">
         <f t="shared" si="6"/>
-        <v>956.94263999999998</v>
+        <v>1357.5232800000001</v>
       </c>
       <c r="F36" s="26"/>
     </row>
@@ -1690,19 +1690,19 @@
       </c>
       <c r="B37" s="19">
         <f>SUM(B28:B36)</f>
-        <v>12356.400000000001</v>
+        <v>11909</v>
       </c>
       <c r="C37" s="19">
         <f>SUM(C28:C36)</f>
-        <v>12727.092000000004</v>
+        <v>14185.438100000001</v>
       </c>
       <c r="D37" s="19">
         <f>SUM(D28:D36)</f>
-        <v>15085.647903000003</v>
+        <v>12634.258100000001</v>
       </c>
       <c r="E37" s="18">
         <f t="shared" si="6"/>
-        <v>40169.13990300001</v>
+        <v>38728.696199999998</v>
       </c>
       <c r="F37" s="29"/>
       <c r="H37" s="29"/>
@@ -1720,19 +1720,19 @@
       </c>
       <c r="B39" s="19">
         <f>SUM(B11,B25,B37)</f>
-        <v>99360.844444444432</v>
+        <v>99449</v>
       </c>
       <c r="C39" s="19">
         <f>SUM(C11,C25,C37)</f>
-        <v>102341.66977777779</v>
+        <v>111459.6681</v>
       </c>
       <c r="D39" s="19">
         <f>SUM(D11,D25,D37)</f>
-        <v>114709.93391411113</v>
+        <v>105505.44410000001</v>
       </c>
       <c r="E39" s="18">
         <f>SUM(B39:D39)</f>
-        <v>316412.44813633332</v>
+        <v>316414.11220000003</v>
       </c>
       <c r="F39" s="29"/>
       <c r="G39" s="28"/>
@@ -2220,19 +2220,19 @@
       </c>
       <c r="B71" s="18">
         <f>B11+B25+B37+B44+B55-B51</f>
-        <v>103160.84444444443</v>
+        <v>103249</v>
       </c>
       <c r="C71" s="18">
         <f>C11+C25+C37+C44+C55-C51</f>
-        <v>108141.66977777779</v>
+        <v>117259.6681</v>
       </c>
       <c r="D71" s="18">
         <f>D11+D25+D37+D44+D55-D51</f>
-        <v>120509.93391411113</v>
+        <v>111305.44410000001</v>
       </c>
       <c r="E71" s="18">
         <f>SUM(B71:D71)</f>
-        <v>331812.44813633332</v>
+        <v>331814.11220000003</v>
       </c>
       <c r="F71" s="26"/>
       <c r="G71" s="26"/>
@@ -2251,19 +2251,19 @@
       </c>
       <c r="B73" s="18">
         <f>B11+B25+B37+B44+B55+B69</f>
-        <v>138582.84444444443</v>
+        <v>138671</v>
       </c>
       <c r="C73" s="18">
         <f>C11+C25+C37+C44+C55+C69</f>
-        <v>131935.24977777779</v>
+        <v>141053.2481</v>
       </c>
       <c r="D73" s="18">
         <f>D11+D25+D37+D44+D55+D69</f>
-        <v>144905.31331411112</v>
+        <v>135700.8235</v>
       </c>
       <c r="E73" s="18">
         <f>SUM(B73:D73)</f>
-        <v>415423.40753633331</v>
+        <v>415425.07159999997</v>
       </c>
       <c r="F73" s="26"/>
       <c r="G73" s="26"/>
@@ -2281,19 +2281,19 @@
       </c>
       <c r="B75" s="18">
         <f>B71*0.555</f>
-        <v>57254.268666666663</v>
+        <v>57303.195000000007</v>
       </c>
       <c r="C75" s="18">
         <f>C71*55.5%</f>
-        <v>60018.626726666676</v>
+        <v>65079.115795500002</v>
       </c>
       <c r="D75" s="18">
         <f>D71*55.5%</f>
-        <v>66883.013322331681</v>
+        <v>61774.521475500012</v>
       </c>
       <c r="E75" s="18">
         <f>SUM(B75:D75)</f>
-        <v>184155.90871566502</v>
+        <v>184156.83227100002</v>
       </c>
       <c r="F75" s="25"/>
       <c r="G75" s="25"/>
@@ -2312,19 +2312,19 @@
       </c>
       <c r="B77" s="18">
         <f>B73+B75</f>
-        <v>195837.1131111111</v>
+        <v>195974.19500000001</v>
       </c>
       <c r="C77" s="18">
         <f>C73+C75</f>
-        <v>191953.87650444446</v>
+        <v>206132.36389549999</v>
       </c>
       <c r="D77" s="18">
         <f>D73+D75</f>
-        <v>211788.3266364428</v>
+        <v>197475.34497550002</v>
       </c>
       <c r="E77" s="18">
         <f>SUM(B77:D77)</f>
-        <v>599579.3162519983</v>
+        <v>599581.90387100005</v>
       </c>
       <c r="F77" s="25"/>
       <c r="G77" s="25"/>

</xml_diff>

<commit_message>
updates to CSSI 2019 budget
</commit_message>
<xml_diff>
--- a/CSSI_2019/forms/CSSI_2019_Budget_AmyRoberts.xlsx
+++ b/CSSI_2019/forms/CSSI_2019_Budget_AmyRoberts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canto\Repositories\SI2.git\CSSI_2019\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6BC409-0F05-4734-8EB8-9822AA2BFE24}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A7E8A5-8EC7-4C47-AA07-AC7EFDDC8C89}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -934,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1031,16 +1031,16 @@
         <v>0</v>
       </c>
       <c r="C8" s="21">
-        <f>$K8*1.03*1.03*10%*1</f>
-        <v>7108.0300000000007</v>
+        <f>$K8*1.03*1.03*10%*0</f>
+        <v>0</v>
       </c>
       <c r="D8" s="21">
-        <f>$K8*1.03*1.03*1.03*10%*0</f>
-        <v>0</v>
+        <f>$K8*1.03*1.03*1.03*10%*1</f>
+        <v>7321.2709000000004</v>
       </c>
       <c r="E8" s="18">
         <f t="shared" ref="E8:E11" si="0">SUM(B8:D8)</f>
-        <v>7108.0300000000007</v>
+        <v>7321.2709000000004</v>
       </c>
       <c r="F8" s="26"/>
       <c r="K8" s="17">
@@ -1076,20 +1076,20 @@
         <v>84</v>
       </c>
       <c r="B10" s="21">
-        <f>K9*(1/10)</f>
-        <v>6700</v>
+        <f>K9*(0.5/9)</f>
+        <v>3722.2222222222222</v>
       </c>
       <c r="C10" s="21">
         <f t="shared" si="1"/>
-        <v>6901</v>
+        <v>3833.8888888888891</v>
       </c>
       <c r="D10" s="21">
         <f t="shared" si="1"/>
-        <v>7108.03</v>
+        <v>3948.905555555556</v>
       </c>
       <c r="E10" s="18">
         <f t="shared" si="0"/>
-        <v>20709.03</v>
+        <v>11505.016666666666</v>
       </c>
       <c r="F10" s="26"/>
     </row>
@@ -1099,19 +1099,19 @@
       </c>
       <c r="B11" s="19">
         <f>SUM(B8:B10)</f>
-        <v>6700</v>
+        <v>3722.2222222222222</v>
       </c>
       <c r="C11" s="19">
         <f>SUM(C8:C10)</f>
-        <v>14009.03</v>
+        <v>3833.8888888888891</v>
       </c>
       <c r="D11" s="19">
         <f>SUM(D8:D10)</f>
-        <v>7108.03</v>
+        <v>11270.176455555556</v>
       </c>
       <c r="E11" s="18">
         <f t="shared" si="0"/>
-        <v>27817.059999999998</v>
+        <v>18826.287566666666</v>
       </c>
       <c r="F11" s="26"/>
     </row>
@@ -1489,19 +1489,19 @@
       </c>
       <c r="B28" s="18">
         <f>B11*27%</f>
-        <v>1809.0000000000002</v>
+        <v>1005</v>
       </c>
       <c r="C28" s="18">
         <f>C11*27%</f>
-        <v>3782.4381000000003</v>
+        <v>1035.1500000000001</v>
       </c>
       <c r="D28" s="18">
         <f>D11*27%</f>
-        <v>1919.1681000000001</v>
+        <v>3042.9476430000004</v>
       </c>
       <c r="E28" s="18">
         <f t="shared" ref="E28:E37" si="6">SUM(B28:D28)</f>
-        <v>7510.6062000000002</v>
+        <v>5083.097643000001</v>
       </c>
       <c r="F28" s="25"/>
     </row>
@@ -1690,19 +1690,19 @@
       </c>
       <c r="B37" s="19">
         <f>SUM(B28:B36)</f>
-        <v>11909</v>
+        <v>11105</v>
       </c>
       <c r="C37" s="19">
         <f>SUM(C28:C36)</f>
-        <v>14185.438100000001</v>
+        <v>11438.150000000001</v>
       </c>
       <c r="D37" s="19">
         <f>SUM(D28:D36)</f>
-        <v>12634.258100000001</v>
+        <v>13758.037643000001</v>
       </c>
       <c r="E37" s="18">
         <f t="shared" si="6"/>
-        <v>38728.696199999998</v>
+        <v>36301.187643000005</v>
       </c>
       <c r="F37" s="29"/>
       <c r="H37" s="29"/>
@@ -1720,19 +1720,19 @@
       </c>
       <c r="B39" s="19">
         <f>SUM(B11,B25,B37)</f>
-        <v>99449</v>
+        <v>95667.222222222219</v>
       </c>
       <c r="C39" s="19">
         <f>SUM(C11,C25,C37)</f>
-        <v>111459.6681</v>
+        <v>98537.238888888882</v>
       </c>
       <c r="D39" s="19">
         <f>SUM(D11,D25,D37)</f>
-        <v>105505.44410000001</v>
+        <v>110791.37009855556</v>
       </c>
       <c r="E39" s="18">
         <f>SUM(B39:D39)</f>
-        <v>316414.11220000003</v>
+        <v>304995.83120966668</v>
       </c>
       <c r="F39" s="29"/>
       <c r="G39" s="28"/>
@@ -2220,19 +2220,19 @@
       </c>
       <c r="B71" s="18">
         <f>B11+B25+B37+B44+B55-B51</f>
-        <v>103249</v>
+        <v>99467.222222222219</v>
       </c>
       <c r="C71" s="18">
         <f>C11+C25+C37+C44+C55-C51</f>
-        <v>117259.6681</v>
+        <v>104337.23888888888</v>
       </c>
       <c r="D71" s="18">
         <f>D11+D25+D37+D44+D55-D51</f>
-        <v>111305.44410000001</v>
+        <v>116591.37009855556</v>
       </c>
       <c r="E71" s="18">
         <f>SUM(B71:D71)</f>
-        <v>331814.11220000003</v>
+        <v>320395.83120966668</v>
       </c>
       <c r="F71" s="26"/>
       <c r="G71" s="26"/>
@@ -2251,19 +2251,19 @@
       </c>
       <c r="B73" s="18">
         <f>B11+B25+B37+B44+B55+B69</f>
-        <v>138671</v>
+        <v>134889.22222222222</v>
       </c>
       <c r="C73" s="18">
         <f>C11+C25+C37+C44+C55+C69</f>
-        <v>141053.2481</v>
+        <v>128130.81888888888</v>
       </c>
       <c r="D73" s="18">
         <f>D11+D25+D37+D44+D55+D69</f>
-        <v>135700.8235</v>
+        <v>140986.74949855555</v>
       </c>
       <c r="E73" s="18">
         <f>SUM(B73:D73)</f>
-        <v>415425.07159999997</v>
+        <v>404006.79060966667</v>
       </c>
       <c r="F73" s="26"/>
       <c r="G73" s="26"/>
@@ -2281,19 +2281,19 @@
       </c>
       <c r="B75" s="18">
         <f>B71*0.555</f>
-        <v>57303.195000000007</v>
+        <v>55204.308333333334</v>
       </c>
       <c r="C75" s="18">
         <f>C71*55.5%</f>
-        <v>65079.115795500002</v>
+        <v>57907.167583333336</v>
       </c>
       <c r="D75" s="18">
         <f>D71*55.5%</f>
-        <v>61774.521475500012</v>
+        <v>64708.210404698344</v>
       </c>
       <c r="E75" s="18">
         <f>SUM(B75:D75)</f>
-        <v>184156.83227100002</v>
+        <v>177819.68632136501</v>
       </c>
       <c r="F75" s="25"/>
       <c r="G75" s="25"/>
@@ -2312,19 +2312,19 @@
       </c>
       <c r="B77" s="18">
         <f>B73+B75</f>
-        <v>195974.19500000001</v>
+        <v>190093.53055555554</v>
       </c>
       <c r="C77" s="18">
         <f>C73+C75</f>
-        <v>206132.36389549999</v>
+        <v>186037.98647222223</v>
       </c>
       <c r="D77" s="18">
         <f>D73+D75</f>
-        <v>197475.34497550002</v>
+        <v>205694.95990325388</v>
       </c>
       <c r="E77" s="18">
         <f>SUM(B77:D77)</f>
-        <v>599581.90387100005</v>
+        <v>581826.47693103156</v>
       </c>
       <c r="F77" s="25"/>
       <c r="G77" s="25"/>

</xml_diff>

<commit_message>
decent budget draft for CSSI 2019
</commit_message>
<xml_diff>
--- a/CSSI_2019/forms/CSSI_2019_Budget_AmyRoberts.xlsx
+++ b/CSSI_2019/forms/CSSI_2019_Budget_AmyRoberts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canto\Repositories\SI2.git\CSSI_2019\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A7E8A5-8EC7-4C47-AA07-AC7EFDDC8C89}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C27AA2B-F4C7-439B-B484-5532F57A0F08}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -935,7 +935,7 @@
   <dimension ref="A1:N129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1168,24 +1168,24 @@
       </c>
       <c r="B15" s="9">
         <f>K15*0.8</f>
-        <v>33600</v>
+        <v>34400</v>
       </c>
       <c r="C15" s="9">
         <f t="shared" ref="C15:D16" si="3">(B15*3%)+B15</f>
-        <v>34608</v>
+        <v>35432</v>
       </c>
       <c r="D15" s="9">
         <f t="shared" si="3"/>
-        <v>35646.239999999998</v>
+        <v>36494.959999999999</v>
       </c>
       <c r="E15" s="18">
         <f t="shared" si="2"/>
-        <v>103854.23999999999</v>
+        <v>106326.95999999999</v>
       </c>
       <c r="H15" s="32"/>
       <c r="I15" s="26"/>
       <c r="K15" s="17">
-        <v>42000</v>
+        <v>43000</v>
       </c>
       <c r="L15" t="s">
         <v>81</v>
@@ -1236,14 +1236,15 @@
         <v>85</v>
       </c>
       <c r="B18" s="9">
+        <f>K18*0</f>
         <v>0</v>
       </c>
       <c r="C18" s="9">
-        <f>K18*0</f>
+        <f>B18*1.03</f>
         <v>0</v>
       </c>
       <c r="D18" s="9">
-        <f>47844*0</f>
+        <f>C18*1.03</f>
         <v>0</v>
       </c>
       <c r="E18" s="18">
@@ -1253,7 +1254,7 @@
       <c r="F18" s="31"/>
       <c r="G18" s="31"/>
       <c r="K18" s="17">
-        <v>47484</v>
+        <v>474484</v>
       </c>
       <c r="L18" t="s">
         <v>76</v>
@@ -1451,19 +1452,19 @@
       </c>
       <c r="B25" s="19">
         <f>SUM(B14:B24)</f>
-        <v>80840</v>
+        <v>81640</v>
       </c>
       <c r="C25" s="19">
         <f>SUM(C14:C24)</f>
-        <v>83265.2</v>
+        <v>84089.2</v>
       </c>
       <c r="D25" s="19">
         <f>SUM(D14:D24)</f>
-        <v>85763.156000000003</v>
+        <v>86611.876000000004</v>
       </c>
       <c r="E25" s="18">
         <f t="shared" si="2"/>
-        <v>249868.35600000003</v>
+        <v>252341.076</v>
       </c>
       <c r="G25" s="28"/>
     </row>
@@ -1511,19 +1512,19 @@
       </c>
       <c r="B29" s="18">
         <f>SUM(B14+B15)*28%</f>
-        <v>9408</v>
+        <v>9632.0000000000018</v>
       </c>
       <c r="C29" s="18">
         <f>SUM(C14+C15)*28%</f>
-        <v>9690.2400000000016</v>
+        <v>9920.9600000000009</v>
       </c>
       <c r="D29" s="18">
         <f>SUM(D14+D15)*28%</f>
-        <v>9980.9472000000005</v>
+        <v>10218.588800000001</v>
       </c>
       <c r="E29" s="18">
         <f t="shared" si="6"/>
-        <v>29079.1872</v>
+        <v>29771.548800000004</v>
       </c>
       <c r="H29" s="32"/>
       <c r="I29" s="26"/>
@@ -1690,19 +1691,19 @@
       </c>
       <c r="B37" s="19">
         <f>SUM(B28:B36)</f>
-        <v>11105</v>
+        <v>11329.000000000002</v>
       </c>
       <c r="C37" s="19">
         <f>SUM(C28:C36)</f>
-        <v>11438.150000000001</v>
+        <v>11668.87</v>
       </c>
       <c r="D37" s="19">
         <f>SUM(D28:D36)</f>
-        <v>13758.037643000001</v>
+        <v>13995.679243</v>
       </c>
       <c r="E37" s="18">
         <f t="shared" si="6"/>
-        <v>36301.187643000005</v>
+        <v>36993.549243000001</v>
       </c>
       <c r="F37" s="29"/>
       <c r="H37" s="29"/>
@@ -1720,19 +1721,19 @@
       </c>
       <c r="B39" s="19">
         <f>SUM(B11,B25,B37)</f>
-        <v>95667.222222222219</v>
+        <v>96691.222222222219</v>
       </c>
       <c r="C39" s="19">
         <f>SUM(C11,C25,C37)</f>
-        <v>98537.238888888882</v>
+        <v>99591.958888888883</v>
       </c>
       <c r="D39" s="19">
         <f>SUM(D11,D25,D37)</f>
-        <v>110791.37009855556</v>
+        <v>111877.73169855557</v>
       </c>
       <c r="E39" s="18">
         <f>SUM(B39:D39)</f>
-        <v>304995.83120966668</v>
+        <v>308160.91280966665</v>
       </c>
       <c r="F39" s="29"/>
       <c r="G39" s="28"/>
@@ -1759,17 +1760,17 @@
         <v>23</v>
       </c>
       <c r="B42" s="24">
-        <v>1200</v>
+        <v>3220</v>
       </c>
       <c r="C42" s="24">
-        <v>1200</v>
+        <v>3220</v>
       </c>
       <c r="D42" s="24">
-        <v>1200</v>
+        <v>3220</v>
       </c>
       <c r="E42" s="18">
         <f>SUM(B42:D42)</f>
-        <v>3600</v>
+        <v>9660</v>
       </c>
       <c r="F42" s="27"/>
       <c r="G42" s="27"/>
@@ -1792,19 +1793,19 @@
       </c>
       <c r="B44" s="19">
         <f>SUM(B42:B43)</f>
-        <v>1200</v>
+        <v>3220</v>
       </c>
       <c r="C44" s="19">
         <f>SUM(C42:C43)</f>
-        <v>1200</v>
+        <v>3220</v>
       </c>
       <c r="D44" s="19">
         <f>SUM(D42:D43)</f>
-        <v>1200</v>
+        <v>3220</v>
       </c>
       <c r="E44" s="18">
         <f>SUM(B44:D44)</f>
-        <v>3600</v>
+        <v>9660</v>
       </c>
       <c r="F44" s="30"/>
       <c r="G44" s="30"/>
@@ -2042,18 +2043,12 @@
       <c r="A62" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B62" s="9">
-        <v>10000</v>
-      </c>
-      <c r="C62" s="9">
-        <v>10000</v>
-      </c>
-      <c r="D62" s="9">
-        <v>10000</v>
-      </c>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
       <c r="E62" s="18">
         <f>SUM(B62:D62)</f>
-        <v>30000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
@@ -2072,24 +2067,36 @@
       <c r="A64" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
+      <c r="B64" s="9">
+        <v>2000</v>
+      </c>
+      <c r="C64" s="9">
+        <v>2000</v>
+      </c>
+      <c r="D64" s="9">
+        <v>2000</v>
+      </c>
       <c r="E64" s="18">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B65" s="9"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9"/>
+      <c r="B65" s="9">
+        <v>8000</v>
+      </c>
+      <c r="C65" s="9">
+        <v>8000</v>
+      </c>
+      <c r="D65" s="9">
+        <v>8000</v>
+      </c>
       <c r="E65" s="18">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>24000</v>
       </c>
       <c r="K65" t="s">
         <v>92</v>
@@ -2220,19 +2227,19 @@
       </c>
       <c r="B71" s="18">
         <f>B11+B25+B37+B44+B55-B51</f>
-        <v>99467.222222222219</v>
+        <v>102511.22222222222</v>
       </c>
       <c r="C71" s="18">
         <f>C11+C25+C37+C44+C55-C51</f>
-        <v>104337.23888888888</v>
+        <v>107411.95888888888</v>
       </c>
       <c r="D71" s="18">
         <f>D11+D25+D37+D44+D55-D51</f>
-        <v>116591.37009855556</v>
+        <v>119697.73169855557</v>
       </c>
       <c r="E71" s="18">
         <f>SUM(B71:D71)</f>
-        <v>320395.83120966668</v>
+        <v>329620.91280966665</v>
       </c>
       <c r="F71" s="26"/>
       <c r="G71" s="26"/>
@@ -2251,19 +2258,19 @@
       </c>
       <c r="B73" s="18">
         <f>B11+B25+B37+B44+B55+B69</f>
-        <v>134889.22222222222</v>
+        <v>137933.22222222222</v>
       </c>
       <c r="C73" s="18">
         <f>C11+C25+C37+C44+C55+C69</f>
-        <v>128130.81888888888</v>
+        <v>131205.53888888887</v>
       </c>
       <c r="D73" s="18">
         <f>D11+D25+D37+D44+D55+D69</f>
-        <v>140986.74949855555</v>
+        <v>144093.11109855556</v>
       </c>
       <c r="E73" s="18">
         <f>SUM(B73:D73)</f>
-        <v>404006.79060966667</v>
+        <v>413231.87220966665</v>
       </c>
       <c r="F73" s="26"/>
       <c r="G73" s="26"/>
@@ -2281,19 +2288,19 @@
       </c>
       <c r="B75" s="18">
         <f>B71*0.555</f>
-        <v>55204.308333333334</v>
+        <v>56893.72833333334</v>
       </c>
       <c r="C75" s="18">
         <f>C71*55.5%</f>
-        <v>57907.167583333336</v>
+        <v>59613.637183333332</v>
       </c>
       <c r="D75" s="18">
         <f>D71*55.5%</f>
-        <v>64708.210404698344</v>
+        <v>66432.241092698343</v>
       </c>
       <c r="E75" s="18">
         <f>SUM(B75:D75)</f>
-        <v>177819.68632136501</v>
+        <v>182939.60660936503</v>
       </c>
       <c r="F75" s="25"/>
       <c r="G75" s="25"/>
@@ -2312,19 +2319,19 @@
       </c>
       <c r="B77" s="18">
         <f>B73+B75</f>
-        <v>190093.53055555554</v>
+        <v>194826.95055555555</v>
       </c>
       <c r="C77" s="18">
         <f>C73+C75</f>
-        <v>186037.98647222223</v>
+        <v>190819.17607222221</v>
       </c>
       <c r="D77" s="18">
         <f>D73+D75</f>
-        <v>205694.95990325388</v>
+        <v>210525.35219125391</v>
       </c>
       <c r="E77" s="18">
         <f>SUM(B77:D77)</f>
-        <v>581826.47693103156</v>
+        <v>596171.47881903173</v>
       </c>
       <c r="F77" s="25"/>
       <c r="G77" s="25"/>

</xml_diff>